<commit_message>
Add clean inequality data
</commit_message>
<xml_diff>
--- a/data/raw-data/gender/gender index data/Gender_Inequality_Index.xlsx
+++ b/data/raw-data/gender/gender index data/Gender_Inequality_Index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admir.jahic\Desktop\HDRO\HDR 2021\Web materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitanyashekar/Desktop/512 Project/512-project-group-10/data/raw-data/gender/gender index data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCCB13F3-28EC-4E7F-BCB3-D4669B12AEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E220DC71-539C-764E-9A01-DBFE6A24CE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 5" sheetId="6" r:id="rId1"/>
@@ -1670,6 +1670,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1693,9 +1696,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2021,12 +2021,12 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B268" sqref="B268"/>
       <selection pane="bottomLeft" activeCell="B268" sqref="B268"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" style="10"/>
+    <col min="1" max="1" width="8.83203125" style="10"/>
     <col min="2" max="2" width="32" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2" style="10" bestFit="1" customWidth="1"/>
@@ -2046,10 +2046,10 @@
     <col min="18" max="18" width="2" style="10" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" style="10" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="2" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.77734375" style="10"/>
+    <col min="21" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="29" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="29" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="36" t="s">
         <v>320</v>
       </c>
@@ -2057,10 +2057,10 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="29" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:20" s="16" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="16" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="29"/>
       <c r="G3" s="31" t="s">
         <v>250</v>
@@ -2071,13 +2071,13 @@
       <c r="K3" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-    </row>
-    <row r="4" spans="1:20" s="29" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+    </row>
+    <row r="4" spans="1:20" s="29" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="C4" s="17" t="s">
         <v>253</v>
       </c>
@@ -2108,24 +2108,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="29" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="41" t="s">
+    <row r="5" spans="1:20" s="29" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C5" s="42" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="23"/>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="42" t="s">
         <v>259</v>
       </c>
       <c r="F5" s="16"/>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="44" t="s">
         <v>260</v>
       </c>
       <c r="H5" s="16"/>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="44" t="s">
         <v>261</v>
       </c>
       <c r="J5" s="16"/>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="44" t="s">
         <v>262</v>
       </c>
       <c r="L5" s="16"/>
@@ -2141,22 +2141,22 @@
       <c r="R5" s="25"/>
       <c r="S5" s="25"/>
     </row>
-    <row r="6" spans="1:20" s="29" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="29" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="30" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="23"/>
-      <c r="E6" s="42"/>
+      <c r="E6" s="43"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="44"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="16"/>
-      <c r="I6" s="44"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="16"/>
-      <c r="K6" s="44"/>
+      <c r="K6" s="45"/>
       <c r="L6" s="16"/>
       <c r="M6" s="26" t="s">
         <v>246</v>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="T6" s="27"/>
     </row>
-    <row r="7" spans="1:20" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="29" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="15"/>
       <c r="B7" s="30"/>
       <c r="C7" s="23">
@@ -2218,31 +2218,31 @@
       </c>
       <c r="T7" s="11"/>
     </row>
-    <row r="8" spans="1:20" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="29"/>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
-      <c r="R8" s="37"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="37"/>
-    </row>
-    <row r="9" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="38"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="38"/>
+      <c r="T8" s="38"/>
+    </row>
+    <row r="9" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="14">
         <v>1</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>72.704999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="14">
         <v>2</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>71.95</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" s="14">
         <v>3</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>70.462999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="14">
         <v>4</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>65.771000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="14">
         <v>5</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>70.546999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="14">
         <v>6</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>66.653000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="14">
         <v>7</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>68.009</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="14">
         <v>8</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>68.572999999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="14">
         <v>9</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>66.040999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="14">
         <v>10</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>71.314999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="14">
         <v>11</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>64.028999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="14">
         <v>12</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>76.828000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="14">
         <v>13</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>58.811999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="14">
         <v>13</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>75.33</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="14">
         <v>15</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>69.741</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="14">
         <v>16</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="14">
         <v>17</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>65.543999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="14">
         <v>18</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>67.090999999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="14">
         <v>19</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>71.031000000000006</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="14">
         <v>19</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>72.447999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="14">
         <v>21</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>66.436999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="14">
         <v>22</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>66.075000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="14">
         <v>23</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>71.412999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="14">
         <v>23</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>62.188000000000002</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="14">
         <v>25</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>66.283000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="14">
         <v>26</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>88.003</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="14">
         <v>27</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>62.411999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="14">
         <v>28</v>
       </c>
@@ -3264,7 +3264,7 @@
         <v>59.674999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="14">
         <v>29</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>68.766000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="14">
         <v>30</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>57.591999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="14">
         <v>31</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>70.168999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="14">
         <v>32</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>68.063999999999993</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="14">
         <v>33</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>58.107999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="14">
         <v>34</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>65.489000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="14">
         <v>35</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>83.531000000000006</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="14">
         <v>35</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>67.864999999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="14">
         <v>35</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>80.146000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="14">
         <v>38</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>62.207999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A47" s="14">
         <v>39</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>66.826999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A48" s="14">
         <v>40</v>
       </c>
@@ -3696,7 +3696,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A49" s="14">
         <v>40</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>58.750999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A50" s="14">
         <v>42</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>65.546999999999997</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A51" s="14">
         <v>42</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>95.456000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A52" s="14">
         <v>44</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="14">
         <v>45</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>66.415000000000006</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="14">
         <v>46</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>67.209999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A55" s="14">
         <v>47</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>71.602999999999994</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" s="14">
         <v>48</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>69.406999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A57" s="14">
         <v>49</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>62.006</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A58" s="14">
         <v>50</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>83.804000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="14">
         <v>51</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>72.338999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A60" s="14">
         <v>52</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>69.716999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="14">
         <v>53</v>
       </c>
@@ -4193,7 +4193,7 @@
         <v>62.34</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A62" s="14">
         <v>54</v>
       </c>
@@ -4228,7 +4228,7 @@
         <v>85.042000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A63" s="14">
         <v>55</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>71.486000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A64" s="14">
         <v>56</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>75.518000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A65" s="14">
         <v>57</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>67.960999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A66" s="14">
         <v>58</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>71.141999999999996</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A67" s="14">
         <v>58</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>69.25</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A68" s="14">
         <v>60</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>71.387</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="14">
         <v>61</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>72.572000000000003</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A70" s="14">
         <v>62</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>77.551000000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A71" s="14">
         <v>63</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>68.03</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A72" s="14">
         <v>63</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>70.447999999999993</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A73" s="14">
         <v>63</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>62.271999999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A74" s="14">
         <v>66</v>
       </c>
@@ -4672,31 +4672,31 @@
         <v>75.027000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:20" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A75" s="4"/>
-      <c r="B75" s="38" t="s">
+      <c r="B75" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C75" s="39"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="39"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="39"/>
-      <c r="J75" s="39"/>
-      <c r="K75" s="39"/>
-      <c r="L75" s="39"/>
-      <c r="M75" s="39"/>
-      <c r="N75" s="39"/>
-      <c r="O75" s="39"/>
-      <c r="P75" s="39"/>
-      <c r="Q75" s="39"/>
-      <c r="R75" s="39"/>
-      <c r="S75" s="39"/>
-      <c r="T75" s="39"/>
-    </row>
-    <row r="76" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
+      <c r="E75" s="40"/>
+      <c r="F75" s="40"/>
+      <c r="G75" s="40"/>
+      <c r="H75" s="40"/>
+      <c r="I75" s="40"/>
+      <c r="J75" s="40"/>
+      <c r="K75" s="40"/>
+      <c r="L75" s="40"/>
+      <c r="M75" s="40"/>
+      <c r="N75" s="40"/>
+      <c r="O75" s="40"/>
+      <c r="P75" s="40"/>
+      <c r="Q75" s="40"/>
+      <c r="R75" s="40"/>
+      <c r="S75" s="40"/>
+      <c r="T75" s="40"/>
+    </row>
+    <row r="76" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A76" s="14">
         <v>67</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>66.153999999999996</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A77" s="14">
         <v>68</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>62.636000000000003</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A78" s="14">
         <v>68</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A79" s="14">
         <v>70</v>
       </c>
@@ -4848,7 +4848,7 @@
         <v>63.726999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A80" s="14">
         <v>71</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="81" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A81" s="14">
         <v>72</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A82" s="14">
         <v>73</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>68.495000000000005</v>
       </c>
     </row>
-    <row r="83" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A83" s="14">
         <v>74</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>52.350999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A84" s="14">
         <v>75</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A85" s="14">
         <v>76</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>68.085999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A86" s="14">
         <v>77</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>63.567</v>
       </c>
     </row>
-    <row r="87" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A87" s="14">
         <v>78</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>63.444000000000003</v>
       </c>
     </row>
-    <row r="88" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A88" s="14">
         <v>79</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>74.290000000000006</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A89" s="14">
         <v>80</v>
       </c>
@@ -5222,7 +5222,7 @@
         <v>75.162000000000006</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A90" s="14">
         <v>80</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>43.932000000000002</v>
       </c>
     </row>
-    <row r="91" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A91" s="14">
         <v>80</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="92" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A92" s="14">
         <v>83</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>68.453999999999994</v>
       </c>
     </row>
-    <row r="93" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A93" s="14">
         <v>84</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>81.875</v>
       </c>
     </row>
-    <row r="94" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A94" s="14">
         <v>85</v>
       </c>
@@ -5409,7 +5409,7 @@
         <v>63.003999999999998</v>
       </c>
     </row>
-    <row r="95" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A95" s="14">
         <v>86</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>75.415000000000006</v>
       </c>
     </row>
-    <row r="96" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A96" s="14">
         <v>87</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>68.239999999999995</v>
       </c>
     </row>
-    <row r="97" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A97" s="14">
         <v>88</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>77.998000000000005</v>
       </c>
     </row>
-    <row r="98" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A98" s="14">
         <v>89</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>74.099999999999994</v>
       </c>
     </row>
-    <row r="99" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A99" s="14">
         <v>90</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>67.494</v>
       </c>
     </row>
-    <row r="100" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A100" s="14">
         <v>91</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>64.48</v>
       </c>
     </row>
-    <row r="101" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A101" s="14">
         <v>91</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>67.341999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A102" s="14">
         <v>91</v>
       </c>
@@ -5716,7 +5716,7 @@
         <v>55.262999999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A103" s="14">
         <v>91</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>55.59</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A104" s="14">
         <v>95</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>76.519000000000005</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A105" s="14">
         <v>96</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>66.572000000000003</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A106" s="14">
         <v>97</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>67.087999999999994</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A107" s="14">
         <v>97</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>67.150000000000006</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A108" s="14">
         <v>99</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>75.257000000000005</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A109" s="14">
         <v>99</v>
       </c>
@@ -5985,7 +5985,7 @@
         <v>65.064999999999998</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A110" s="14">
         <v>101</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>70.915999999999997</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A111" s="14">
         <v>102</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A112" s="14">
         <v>102</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>62.322000000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A113" s="14">
         <v>104</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>60.969000000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A114" s="14">
         <v>105</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>84.213999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A115" s="14">
         <v>106</v>
       </c>
@@ -6201,7 +6201,7 @@
         <v>66.286000000000001</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A116" s="14">
         <v>106</v>
       </c>
@@ -6236,7 +6236,7 @@
         <v>73.227999999999994</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A117" s="14">
         <v>108</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>64.096999999999994</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A118" s="14">
         <v>109</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>59.883000000000003</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A119" s="14">
         <v>110</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>70.003</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A120" s="14">
         <v>111</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>54.237000000000002</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A121" s="14">
         <v>112</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>57.012</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A122" s="14">
         <v>112</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>64.331999999999994</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A123" s="14">
         <v>114</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>81.668000000000006</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A124" s="14">
         <v>115</v>
       </c>
@@ -6543,31 +6543,31 @@
         <v>79.436999999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:20" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A125" s="4"/>
-      <c r="B125" s="38" t="s">
+      <c r="B125" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="C125" s="38"/>
-      <c r="D125" s="38"/>
-      <c r="E125" s="38"/>
-      <c r="F125" s="38"/>
-      <c r="G125" s="38"/>
-      <c r="H125" s="38"/>
-      <c r="I125" s="38"/>
-      <c r="J125" s="38"/>
-      <c r="K125" s="38"/>
-      <c r="L125" s="38"/>
-      <c r="M125" s="38"/>
-      <c r="N125" s="38"/>
-      <c r="O125" s="38"/>
-      <c r="P125" s="38"/>
-      <c r="Q125" s="38"/>
-      <c r="R125" s="38"/>
-      <c r="S125" s="38"/>
-      <c r="T125" s="38"/>
-    </row>
-    <row r="126" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C125" s="39"/>
+      <c r="D125" s="39"/>
+      <c r="E125" s="39"/>
+      <c r="F125" s="39"/>
+      <c r="G125" s="39"/>
+      <c r="H125" s="39"/>
+      <c r="I125" s="39"/>
+      <c r="J125" s="39"/>
+      <c r="K125" s="39"/>
+      <c r="L125" s="39"/>
+      <c r="M125" s="39"/>
+      <c r="N125" s="39"/>
+      <c r="O125" s="39"/>
+      <c r="P125" s="39"/>
+      <c r="Q125" s="39"/>
+      <c r="R125" s="39"/>
+      <c r="S125" s="39"/>
+      <c r="T125" s="39"/>
+    </row>
+    <row r="126" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A126" s="14">
         <v>116</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>68.302000000000007</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A127" s="14">
         <v>117</v>
       </c>
@@ -6637,7 +6637,7 @@
         <v>65.147999999999996</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A128" s="14">
         <v>118</v>
       </c>
@@ -6672,7 +6672,7 @@
         <v>83.765000000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A129" s="14">
         <v>118</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>71.67</v>
       </c>
     </row>
-    <row r="130" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A130" s="14">
         <v>120</v>
       </c>
@@ -6754,7 +6754,7 @@
         <v>67.813000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A131" s="14">
         <v>121</v>
       </c>
@@ -6795,7 +6795,7 @@
         <v>71.763000000000005</v>
       </c>
     </row>
-    <row r="132" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A132" s="14">
         <v>122</v>
       </c>
@@ -6836,7 +6836,7 @@
         <v>50.533999999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A133" s="14">
         <v>123</v>
       </c>
@@ -6871,7 +6871,7 @@
         <v>76.751999999999995</v>
       </c>
     </row>
-    <row r="134" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A134" s="14">
         <v>123</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>65.95</v>
       </c>
     </row>
-    <row r="135" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A135" s="14">
         <v>125</v>
       </c>
@@ -6941,7 +6941,7 @@
         <v>72.569999999999993</v>
       </c>
     </row>
-    <row r="136" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A136" s="14">
         <v>126</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>81.299000000000007</v>
       </c>
     </row>
-    <row r="137" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A137" s="14">
         <v>127</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>67.397000000000006</v>
       </c>
     </row>
-    <row r="138" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A138" s="14">
         <v>128</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>61.704999999999998</v>
       </c>
     </row>
-    <row r="139" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A139" s="14">
         <v>129</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>78.781999999999996</v>
       </c>
     </row>
-    <row r="140" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A140" s="14">
         <v>130</v>
       </c>
@@ -7122,7 +7122,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="141" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A141" s="14">
         <v>131</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="142" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A142" s="14">
         <v>132</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>70.091999999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A143" s="14">
         <v>133</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>72.233999999999995</v>
       </c>
     </row>
-    <row r="144" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A144" s="14">
         <v>134</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="145" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A145" s="14">
         <v>135</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>80.268000000000001</v>
       </c>
     </row>
-    <row r="146" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A146" s="14">
         <v>136</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="147" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A147" s="14">
         <v>137</v>
       </c>
@@ -7382,7 +7382,7 @@
         <v>78.94</v>
       </c>
     </row>
-    <row r="148" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A148" s="14">
         <v>138</v>
       </c>
@@ -7423,7 +7423,7 @@
         <v>69.876000000000005</v>
       </c>
     </row>
-    <row r="149" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A149" s="14">
         <v>139</v>
       </c>
@@ -7464,7 +7464,7 @@
         <v>62.180999999999997</v>
       </c>
     </row>
-    <row r="150" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A150" s="14">
         <v>140</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>78.093000000000004</v>
       </c>
     </row>
-    <row r="151" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A151" s="14">
         <v>140</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>72.239999999999995</v>
       </c>
     </row>
-    <row r="152" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A152" s="14">
         <v>140</v>
       </c>
@@ -7572,7 +7572,7 @@
         <v>78.006</v>
       </c>
     </row>
-    <row r="153" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A153" s="14">
         <v>143</v>
       </c>
@@ -7613,7 +7613,7 @@
         <v>80.772000000000006</v>
       </c>
     </row>
-    <row r="154" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A154" s="14">
         <v>144</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>53.606000000000002</v>
       </c>
     </row>
-    <row r="155" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A155" s="14">
         <v>145</v>
       </c>
@@ -7683,7 +7683,7 @@
         <v>58.482999999999997</v>
       </c>
     </row>
-    <row r="156" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A156" s="14">
         <v>146</v>
       </c>
@@ -7718,7 +7718,7 @@
         <v>85.918000000000006</v>
       </c>
     </row>
-    <row r="157" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A157" s="14">
         <v>146</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>88.933000000000007</v>
       </c>
     </row>
-    <row r="158" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A158" s="14">
         <v>148</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>79.070999999999998</v>
       </c>
     </row>
-    <row r="159" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A159" s="14">
         <v>149</v>
       </c>
@@ -7829,7 +7829,7 @@
         <v>69.962000000000003</v>
       </c>
     </row>
-    <row r="160" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A160" s="14">
         <v>150</v>
       </c>
@@ -7870,7 +7870,7 @@
         <v>70.766999999999996</v>
       </c>
     </row>
-    <row r="161" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A161" s="14">
         <v>151</v>
       </c>
@@ -7911,7 +7911,7 @@
         <v>80.747</v>
       </c>
     </row>
-    <row r="162" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A162" s="14">
         <v>152</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>75.563999999999993</v>
       </c>
     </row>
-    <row r="163" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A163" s="14">
         <v>153</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>67.605000000000004</v>
       </c>
     </row>
-    <row r="164" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A164" s="14">
         <v>154</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>77.846999999999994</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A165" s="14">
         <v>155</v>
       </c>
@@ -8063,7 +8063,7 @@
         <v>87.397999999999996</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A166" s="14">
         <v>156</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>54.533999999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A167" s="14">
         <v>156</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>48.14</v>
       </c>
     </row>
-    <row r="168" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A168" s="14">
         <v>158</v>
       </c>
@@ -8177,7 +8177,7 @@
         <v>62.19</v>
       </c>
     </row>
-    <row r="169" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A169" s="14">
         <v>159</v>
       </c>
@@ -8218,31 +8218,31 @@
         <v>64.893000000000001</v>
       </c>
     </row>
-    <row r="170" spans="1:20" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:20" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A170" s="4"/>
-      <c r="B170" s="38" t="s">
+      <c r="B170" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="C170" s="39"/>
-      <c r="D170" s="39"/>
-      <c r="E170" s="39"/>
-      <c r="F170" s="39"/>
-      <c r="G170" s="39"/>
-      <c r="H170" s="39"/>
-      <c r="I170" s="39"/>
-      <c r="J170" s="39"/>
-      <c r="K170" s="39"/>
-      <c r="L170" s="39"/>
-      <c r="M170" s="39"/>
-      <c r="N170" s="39"/>
-      <c r="O170" s="39"/>
-      <c r="P170" s="39"/>
-      <c r="Q170" s="39"/>
-      <c r="R170" s="39"/>
-      <c r="S170" s="39"/>
-      <c r="T170" s="39"/>
-    </row>
-    <row r="171" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="C170" s="40"/>
+      <c r="D170" s="40"/>
+      <c r="E170" s="40"/>
+      <c r="F170" s="40"/>
+      <c r="G170" s="40"/>
+      <c r="H170" s="40"/>
+      <c r="I170" s="40"/>
+      <c r="J170" s="40"/>
+      <c r="K170" s="40"/>
+      <c r="L170" s="40"/>
+      <c r="M170" s="40"/>
+      <c r="N170" s="40"/>
+      <c r="O170" s="40"/>
+      <c r="P170" s="40"/>
+      <c r="Q170" s="40"/>
+      <c r="R170" s="40"/>
+      <c r="S170" s="40"/>
+      <c r="T170" s="40"/>
+    </row>
+    <row r="171" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A171" s="14">
         <v>160</v>
       </c>
@@ -8283,7 +8283,7 @@
         <v>87.097999999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A172" s="14">
         <v>161</v>
       </c>
@@ -8318,7 +8318,7 @@
         <v>78.078999999999994</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A173" s="14">
         <v>162</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>59.369</v>
       </c>
     </row>
-    <row r="174" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A174" s="14">
         <v>163</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>68.930000000000007</v>
       </c>
     </row>
-    <row r="175" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A175" s="14">
         <v>163</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>59.591000000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A176" s="14">
         <v>165</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>82.225999999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A177" s="14">
         <v>166</v>
       </c>
@@ -8520,7 +8520,7 @@
         <v>72.599000000000004</v>
       </c>
     </row>
-    <row r="178" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A178" s="14">
         <v>166</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>71.305999999999997</v>
       </c>
     </row>
-    <row r="179" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A179" s="14">
         <v>168</v>
       </c>
@@ -8596,7 +8596,7 @@
         <v>71.343000000000004</v>
       </c>
     </row>
-    <row r="180" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A180" s="14">
         <v>169</v>
       </c>
@@ -8637,7 +8637,7 @@
         <v>79.953000000000003</v>
       </c>
     </row>
-    <row r="181" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A181" s="14">
         <v>170</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>56.728999999999999</v>
       </c>
     </row>
-    <row r="182" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A182" s="14">
         <v>171</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>44.146999999999998</v>
       </c>
     </row>
-    <row r="183" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A183" s="14">
         <v>172</v>
       </c>
@@ -8751,7 +8751,7 @@
         <v>67.819000000000003</v>
       </c>
     </row>
-    <row r="184" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A184" s="14">
         <v>173</v>
       </c>
@@ -8792,7 +8792,7 @@
         <v>87.594999999999999</v>
       </c>
     </row>
-    <row r="185" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A185" s="14">
         <v>174</v>
       </c>
@@ -8827,7 +8827,7 @@
         <v>66.259</v>
       </c>
     </row>
-    <row r="186" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A186" s="14">
         <v>175</v>
       </c>
@@ -8862,7 +8862,7 @@
         <v>84.683000000000007</v>
       </c>
     </row>
-    <row r="187" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A187" s="14">
         <v>176</v>
       </c>
@@ -8900,7 +8900,7 @@
         <v>83.622</v>
       </c>
     </row>
-    <row r="188" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A188" s="14">
         <v>177</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>78.373000000000005</v>
       </c>
     </row>
-    <row r="189" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A189" s="14">
         <v>178</v>
       </c>
@@ -8970,7 +8970,7 @@
         <v>79.716999999999999</v>
       </c>
     </row>
-    <row r="190" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A190" s="14">
         <v>179</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>69.064999999999998</v>
       </c>
     </row>
-    <row r="191" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="A191" s="14">
         <v>180</v>
       </c>
@@ -9046,7 +9046,7 @@
         <v>66.515000000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:19" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" ht="15" x14ac:dyDescent="0.15">
       <c r="A192" s="14">
         <v>181</v>
       </c>
@@ -9087,7 +9087,7 @@
         <v>55.924999999999997</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A193" s="14">
         <v>182</v>
       </c>
@@ -9131,7 +9131,7 @@
         <v>62.188000000000002</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A194" s="14">
         <v>183</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>67.637</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A195" s="14">
         <v>184</v>
       </c>
@@ -9207,7 +9207,7 @@
         <v>72.724999999999994</v>
       </c>
     </row>
-    <row r="196" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A196" s="14">
         <v>185</v>
       </c>
@@ -9248,7 +9248,7 @@
         <v>78.930999999999997</v>
       </c>
     </row>
-    <row r="197" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A197" s="14">
         <v>186</v>
       </c>
@@ -9283,7 +9283,7 @@
         <v>79.673000000000002</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A198" s="14">
         <v>187</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>77.379000000000005</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A199" s="14">
         <v>188</v>
       </c>
@@ -9359,7 +9359,7 @@
         <v>79.486000000000004</v>
       </c>
     </row>
-    <row r="200" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A200" s="14">
         <v>189</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>84.266999999999996</v>
       </c>
     </row>
-    <row r="201" spans="1:20" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:20" ht="15" x14ac:dyDescent="0.15">
       <c r="A201" s="14">
         <v>190</v>
       </c>
@@ -9441,7 +9441,7 @@
         <v>69.927000000000007</v>
       </c>
     </row>
-    <row r="202" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="A202" s="14">
         <v>191</v>
       </c>
@@ -9476,31 +9476,31 @@
         <v>73.573999999999998</v>
       </c>
     </row>
-    <row r="203" spans="1:20" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:20" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A203" s="29"/>
-      <c r="B203" s="38" t="s">
+      <c r="B203" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="C203" s="39"/>
-      <c r="D203" s="39"/>
-      <c r="E203" s="39"/>
-      <c r="F203" s="39"/>
-      <c r="G203" s="39"/>
-      <c r="H203" s="39"/>
-      <c r="I203" s="39"/>
-      <c r="J203" s="39"/>
-      <c r="K203" s="39"/>
-      <c r="L203" s="39"/>
-      <c r="M203" s="39"/>
-      <c r="N203" s="39"/>
-      <c r="O203" s="39"/>
-      <c r="P203" s="39"/>
-      <c r="Q203" s="39"/>
-      <c r="R203" s="39"/>
-      <c r="S203" s="39"/>
-      <c r="T203" s="39"/>
-    </row>
-    <row r="204" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C203" s="40"/>
+      <c r="D203" s="40"/>
+      <c r="E203" s="40"/>
+      <c r="F203" s="40"/>
+      <c r="G203" s="40"/>
+      <c r="H203" s="40"/>
+      <c r="I203" s="40"/>
+      <c r="J203" s="40"/>
+      <c r="K203" s="40"/>
+      <c r="L203" s="40"/>
+      <c r="M203" s="40"/>
+      <c r="N203" s="40"/>
+      <c r="O203" s="40"/>
+      <c r="P203" s="40"/>
+      <c r="Q203" s="40"/>
+      <c r="R203" s="40"/>
+      <c r="S203" s="40"/>
+      <c r="T203" s="40"/>
+    </row>
+    <row r="204" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="B204" s="7" t="s">
         <v>219</v>
       </c>
@@ -9532,7 +9532,7 @@
         <v>86.141000000000005</v>
       </c>
     </row>
-    <row r="205" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="B205" s="7" t="s">
         <v>221</v>
       </c>
@@ -9564,7 +9564,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="B206" s="7" t="s">
         <v>222</v>
       </c>
@@ -9596,7 +9596,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:20" ht="14" x14ac:dyDescent="0.15">
       <c r="B207" s="7" t="s">
         <v>223</v>
       </c>
@@ -9628,12 +9628,12 @@
         <v>46.978000000000002</v>
       </c>
     </row>
-    <row r="209" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B209" s="1" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="210" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B210" s="9" t="s">
         <v>225</v>
       </c>
@@ -9665,7 +9665,7 @@
         <v>68.41296100282527</v>
       </c>
     </row>
-    <row r="211" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B211" s="9" t="s">
         <v>227</v>
       </c>
@@ -9697,7 +9697,7 @@
         <v>73.475962516413375</v>
       </c>
     </row>
-    <row r="212" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B212" s="9" t="s">
         <v>228</v>
       </c>
@@ -9729,7 +9729,7 @@
         <v>71.304786781173689</v>
       </c>
     </row>
-    <row r="213" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B213" s="9" t="s">
         <v>229</v>
       </c>
@@ -9761,7 +9761,7 @@
         <v>73.208956352524652</v>
       </c>
     </row>
-    <row r="214" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B214" s="9"/>
       <c r="C214" s="12"/>
       <c r="E214" s="4"/>
@@ -9773,7 +9773,7 @@
       <c r="Q214" s="13"/>
       <c r="S214" s="13"/>
     </row>
-    <row r="215" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B215" s="5" t="s">
         <v>230</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>72.766216076112272</v>
       </c>
     </row>
-    <row r="216" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B216" s="9"/>
       <c r="C216" s="12"/>
       <c r="E216" s="4"/>
@@ -9817,7 +9817,7 @@
       <c r="Q216" s="13"/>
       <c r="S216" s="13"/>
     </row>
-    <row r="217" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B217" s="1" t="s">
         <v>231</v>
       </c>
@@ -9831,7 +9831,7 @@
       <c r="Q217" s="13"/>
       <c r="S217" s="13"/>
     </row>
-    <row r="218" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B218" s="9" t="s">
         <v>232</v>
       </c>
@@ -9863,7 +9863,7 @@
         <v>69.466017652920669</v>
       </c>
     </row>
-    <row r="219" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B219" s="9" t="s">
         <v>233</v>
       </c>
@@ -9895,7 +9895,7 @@
         <v>75.209126088685721</v>
       </c>
     </row>
-    <row r="220" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B220" s="9" t="s">
         <v>234</v>
       </c>
@@ -9927,7 +9927,7 @@
         <v>67.038752317145068</v>
       </c>
     </row>
-    <row r="221" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B221" s="9" t="s">
         <v>235</v>
       </c>
@@ -9959,7 +9959,7 @@
         <v>72.656570791922974</v>
       </c>
     </row>
-    <row r="222" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B222" s="9" t="s">
         <v>236</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>71.585598936887578</v>
       </c>
     </row>
-    <row r="223" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B223" s="9" t="s">
         <v>237</v>
       </c>
@@ -10023,7 +10023,7 @@
         <v>72.25366195212041</v>
       </c>
     </row>
-    <row r="224" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B224" s="9"/>
       <c r="C224" s="12"/>
       <c r="E224" s="4"/>
@@ -10035,7 +10035,7 @@
       <c r="Q224" s="13"/>
       <c r="S224" s="13"/>
     </row>
-    <row r="225" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B225" s="5" t="s">
         <v>238</v>
       </c>
@@ -10067,7 +10067,7 @@
         <v>75.799930131532506</v>
       </c>
     </row>
-    <row r="226" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B226" s="1" t="s">
         <v>239</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>68.678533429113685</v>
       </c>
     </row>
-    <row r="227" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B227" s="9"/>
       <c r="C227" s="12"/>
       <c r="E227" s="4"/>
@@ -10111,7 +10111,7 @@
       <c r="Q227" s="13"/>
       <c r="S227" s="13"/>
     </row>
-    <row r="228" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B228" s="1" t="s">
         <v>240</v>
       </c>
@@ -10143,7 +10143,7 @@
         <v>67.778492101429123</v>
       </c>
     </row>
-    <row r="229" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B229" s="9"/>
       <c r="C229" s="12"/>
       <c r="E229" s="4"/>
@@ -10155,7 +10155,7 @@
       <c r="Q229" s="13"/>
       <c r="S229" s="13"/>
     </row>
-    <row r="230" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B230" s="5" t="s">
         <v>241</v>
       </c>
@@ -10187,121 +10187,121 @@
         <v>71.691739741898459</v>
       </c>
     </row>
-    <row r="231" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B231" s="3"/>
     </row>
-    <row r="232" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B232" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="233" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B233" s="7" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="234" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B234" s="7" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="235" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B235" s="7" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="236" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B236" s="7" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="237" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B237" s="7" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="238" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B238" s="7" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="239" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B239" s="7" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="240" spans="2:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B240" s="7" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="241" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B241" s="7" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="242" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B242" s="7" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="243" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B243" s="7" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="244" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B244" s="7" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="245" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B245" s="7" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="246" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B246" s="7" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="247" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B247" s="7" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="248" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B248" s="7" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="249" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B249" s="7" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="250" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B250" s="7" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="251" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B251" s="7" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="252" spans="1:19" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:19" ht="14" x14ac:dyDescent="0.15">
       <c r="B252" s="7" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="254" spans="1:19" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:19" s="29" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A254" s="4"/>
       <c r="B254" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="255" spans="1:19" s="29" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:19" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A255" s="4"/>
       <c r="B255" s="7" t="s">
         <v>321</v>
@@ -10324,108 +10324,108 @@
       <c r="R255" s="7"/>
       <c r="S255" s="7"/>
     </row>
-    <row r="256" spans="1:19" s="29" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:19" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A256" s="4"/>
       <c r="B256" s="1" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="257" spans="1:19" s="29" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:19" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A257" s="4"/>
       <c r="B257" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="258" spans="1:19" s="29" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:19" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A258" s="4"/>
       <c r="B258" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="259" spans="1:19" s="29" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:19" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A259" s="4"/>
       <c r="B259" s="7" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="260" spans="1:19" s="29" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:19" s="29" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A260" s="4"/>
       <c r="B260" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="261" spans="1:19" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25"/>
-    <row r="262" spans="1:19" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:19" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="262" spans="1:19" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B262" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="263" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B263" s="7" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="264" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B264" s="7" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="265" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B265" s="45" t="s">
+    <row r="265" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B265" s="37" t="s">
         <v>271</v>
       </c>
-      <c r="C265" s="45"/>
-      <c r="D265" s="45"/>
-      <c r="E265" s="45"/>
-      <c r="F265" s="45"/>
-      <c r="G265" s="45"/>
-      <c r="H265" s="45"/>
-      <c r="I265" s="45"/>
-      <c r="J265" s="45"/>
-      <c r="K265" s="45"/>
-      <c r="L265" s="45"/>
-      <c r="M265" s="45"/>
-      <c r="N265" s="45"/>
-      <c r="O265" s="45"/>
-      <c r="P265" s="45"/>
-      <c r="Q265" s="45"/>
-      <c r="R265" s="45"/>
-      <c r="S265" s="45"/>
-    </row>
-    <row r="266" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C265" s="37"/>
+      <c r="D265" s="37"/>
+      <c r="E265" s="37"/>
+      <c r="F265" s="37"/>
+      <c r="G265" s="37"/>
+      <c r="H265" s="37"/>
+      <c r="I265" s="37"/>
+      <c r="J265" s="37"/>
+      <c r="K265" s="37"/>
+      <c r="L265" s="37"/>
+      <c r="M265" s="37"/>
+      <c r="N265" s="37"/>
+      <c r="O265" s="37"/>
+      <c r="P265" s="37"/>
+      <c r="Q265" s="37"/>
+      <c r="R265" s="37"/>
+      <c r="S265" s="37"/>
+    </row>
+    <row r="266" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B266" s="7" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="267" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B267" s="7" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="268" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B268" s="7" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="269" spans="1:19" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B269" s="7" t="s">
         <v>274</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="K5:K6"/>
     <mergeCell ref="B265:S265"/>
     <mergeCell ref="B8:T8"/>
     <mergeCell ref="B75:T75"/>
     <mergeCell ref="B125:T125"/>
     <mergeCell ref="B170:T170"/>
     <mergeCell ref="B203:T203"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="cover!A1" display="Back" xr:uid="{41E5C26B-7637-470A-B118-A7F098D9F683}"/>
@@ -10444,136 +10444,136 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="166.88671875" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="8.77734375" style="10"/>
+    <col min="1" max="1" width="166.83203125" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="36" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="33" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="33"/>
     </row>
-    <row r="5" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="34" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="35" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="34" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="34" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="34" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="34" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="34" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="34" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="34" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="34" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="34" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="34" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="34" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="29" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="34" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="34" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="34" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="34" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="34" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="34" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="34" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="34" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="34" t="s">
         <v>313</v>
       </c>
@@ -10601,6 +10601,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AD45DB714643E4A8A8C58D3ECEF2B52" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0377062c7993f79e0ee2fe840fd08d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b0611ad7-5071-45af-a141-b2a079deb018" xmlns:ns3="7f64e6aa-b736-4f26-84cc-faf427629e48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2869b255174fce0a927e36b6c0c9136f" ns2:_="" ns3:_="">
     <xsd:import namespace="b0611ad7-5071-45af-a141-b2a079deb018"/>
@@ -10779,15 +10788,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7DA61EB-8D48-4617-94E1-454D1449F940}">
   <ds:schemaRefs>
@@ -10799,6 +10799,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BAEA50D-A77A-4BD1-A57D-FE81CA4DEB01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E66ED643-5F43-47CB-8288-3F0E93434226}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10815,12 +10823,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2BAEA50D-A77A-4BD1-A57D-FE81CA4DEB01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>